<commit_message>
Commit before running regressions
</commit_message>
<xml_diff>
--- a/Data/StimulusGDPfromABD_COVID policy database.xlsx
+++ b/Data/StimulusGDPfromABD_COVID policy database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/2_SCHOOL/5_PAPERS/COVID19-DOMINANCE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB06860-AF46-4E4F-9FE2-6C622D463351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F7C66-5488-C240-B120-9A3FC22FF238}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23140" windowHeight="21600" xr2:uid="{E8707E3B-65C9-554D-8C90-6A5894CB38A7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23140" windowHeight="21140" xr2:uid="{E8707E3B-65C9-554D-8C90-6A5894CB38A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>